<commit_message>
Converting Intel Process into Re Framework
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/FrameworkTemplates/REFramework/VB/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\603214\Documents\UiPath\Intel Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE544FF6-C3F6-4D8A-A010-FDE557B864E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10248" yWindow="17508" windowWidth="21252" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,45 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>ConfigTesting</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>Config_INTEL_Manual_Login</t>
+  </si>
+  <si>
+    <t>Config_INTEL_Continue</t>
+  </si>
+  <si>
+    <t>INTEL_File_Ready</t>
+  </si>
+  <si>
+    <t>DelayBefore</t>
+  </si>
+  <si>
+    <t>DelayAfter</t>
+  </si>
+  <si>
+    <t>TimeoutMedium</t>
+  </si>
+  <si>
+    <t>TimeoutShort</t>
+  </si>
+  <si>
+    <t>NumberOfRetries</t>
+  </si>
+  <si>
+    <t>RetryInterval</t>
+  </si>
+  <si>
+    <t>00:00:03</t>
+  </si>
+  <si>
+    <t>Config_TSI_ReRun</t>
   </si>
 </sst>
 </file>
@@ -211,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -220,6 +259,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,16 +581,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -594,7 +638,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -604,7 +648,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -615,7 +659,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1619,16 +1670,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1716,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1727,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1841,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1801,16 +1852,78 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="5">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="5">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2786,12 +2899,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>